<commit_message>
add fixed course to schedule
</commit_message>
<xml_diff>
--- a/Course Scheduler/output.xlsx
+++ b/Course Scheduler/output.xlsx
@@ -31,34 +31,43 @@
     <x:t>Times</x:t>
   </x:si>
   <x:si>
+    <x:t>fix</x:t>
+  </x:si>
+  <x:si>
+    <x:t>a132</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">SaturdayT1  everyWeek  </x:t>
+  </x:si>
+  <x:si>
     <x:t>c1</x:t>
   </x:si>
   <x:si>
     <x:t>asdasd</x:t>
   </x:si>
   <x:si>
+    <x:t xml:space="preserve">SunDayT2  everyWeek  SunDayT1  odd  </x:t>
+  </x:si>
+  <x:si>
     <x:t xml:space="preserve">SunDayT1  everyWeek  SunDayT2  odd  </x:t>
   </x:si>
   <x:si>
+    <x:t xml:space="preserve">SunDayT2  everyWeek  SunDayT1  even  </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">SaturdayT2  everyWeek  SaturdayT1  odd  </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">SunDayT1  everyWeek  SunDayT2  even  </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">SaturdayT1  everyWeek  SaturdayT2  even  </x:t>
+  </x:si>
+  <x:si>
     <x:t xml:space="preserve">SaturdayT1  everyWeek  SaturdayT2  odd  </x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">SaturdayT2  everyWeek  SaturdayT1  odd  </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SunDayT1  everyWeek  SunDayT2  even  </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SaturdayT1  everyWeek  SaturdayT2  even  </x:t>
-  </x:si>
-  <x:si>
     <x:t xml:space="preserve">SaturdayT2  everyWeek  SaturdayT1  even  </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SunDayT2  everyWeek  SunDayT1  odd  </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SunDayT2  everyWeek  SunDayT1  even  </x:t>
   </x:si>
 </x:sst>
 </file>
@@ -421,7 +430,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E24"/>
+  <x:dimension ref="A1:E32"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -463,66 +472,80 @@
         <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:5" s="1" customFormat="1">
-      <x:c r="A5" s="1">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="B5" s="1">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:5">
-      <x:c r="C6" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D6" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="E6" s="0" t="s">
+    <x:row r="4" spans="1:5">
+      <x:c r="C4" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-    </x:row>
-    <x:row r="8" spans="1:5" s="1" customFormat="1">
-      <x:c r="A8" s="1">
+      <x:c r="D4" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:5" s="1" customFormat="1">
+      <x:c r="A6" s="1">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B6" s="1">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:5">
+      <x:c r="C7" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:5">
+      <x:c r="C8" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:5" s="1" customFormat="1">
+      <x:c r="A10" s="1">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="B8" s="1">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:5">
-      <x:c r="C9" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D9" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="E9" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:5" s="1" customFormat="1">
-      <x:c r="A11" s="1">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="B11" s="1">
-        <x:v>1</x:v>
+      <x:c r="B10" s="1">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:5">
+      <x:c r="C11" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:5">
       <x:c r="C12" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:5" s="1" customFormat="1">
       <x:c r="A14" s="1">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B14" s="1">
         <x:v>1</x:v>
@@ -536,64 +559,138 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="E15" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:5" s="1" customFormat="1">
-      <x:c r="A17" s="1">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B17" s="1">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:5">
-      <x:c r="C18" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D18" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="E18" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:5" s="1" customFormat="1">
-      <x:c r="A20" s="1">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B20" s="1">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:5">
-      <x:c r="C21" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D21" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="E21" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:5">
+      <x:c r="C16" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
     </x:row>
-    <x:row r="23" spans="1:5" s="1" customFormat="1">
-      <x:c r="A23" s="1">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="B23" s="1">
-        <x:v>1</x:v>
+    <x:row r="18" spans="1:5" s="1" customFormat="1">
+      <x:c r="A18" s="1">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B18" s="1">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:5">
+      <x:c r="C19" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E19" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:5">
+      <x:c r="C20" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E20" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:5" s="1" customFormat="1">
+      <x:c r="A22" s="1">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B22" s="1">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:5">
+      <x:c r="C23" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E23" s="0" t="s">
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:5">
       <x:c r="C24" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D24" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E24" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:5" s="1" customFormat="1">
+      <x:c r="A26" s="1">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B26" s="1">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:5">
+      <x:c r="C27" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E27" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:5">
+      <x:c r="C28" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E28" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:5" s="1" customFormat="1">
+      <x:c r="A30" s="1">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B30" s="1">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:5">
+      <x:c r="C31" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E31" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:5">
+      <x:c r="C32" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D32" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E32" s="0" t="s">
+        <x:v>17</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
add Penalty to navbar
</commit_message>
<xml_diff>
--- a/Course Scheduler/output.xlsx
+++ b/Course Scheduler/output.xlsx
@@ -46,28 +46,28 @@
     <x:t>asdasd</x:t>
   </x:si>
   <x:si>
+    <x:t xml:space="preserve">SunDayT1  everyWeek  SunDayT2  odd  </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">SaturdayT2  everyWeek  SaturdayT1  even  </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">SunDayT2  everyWeek  SunDayT1  even  </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">SaturdayT2  everyWeek  SaturdayT1  odd  </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">SunDayT1  everyWeek  SunDayT2  even  </x:t>
+  </x:si>
+  <x:si>
     <x:t xml:space="preserve">SunDayT2  everyWeek  SunDayT1  odd  </x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">SunDayT1  everyWeek  SunDayT2  odd  </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SunDayT2  everyWeek  SunDayT1  even  </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SaturdayT2  everyWeek  SaturdayT1  odd  </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SunDayT1  everyWeek  SunDayT2  even  </x:t>
+    <x:t xml:space="preserve">SaturdayT1  everyWeek  SaturdayT2  odd  </x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">SaturdayT1  everyWeek  SaturdayT2  even  </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SaturdayT1  everyWeek  SaturdayT2  odd  </x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">SaturdayT2  everyWeek  SaturdayT1  even  </x:t>
   </x:si>
 </x:sst>
 </file>
@@ -638,7 +638,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B26" s="1">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:5">
@@ -668,7 +668,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B30" s="1">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:5">

</xml_diff>